<commit_message>
EPBDS-8660 Support Range arrays in Smart Rules
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8323_Simple_Rules_Ranges_Arrays.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8323_Simple_Rules_Ranges_Arrays.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
   <si>
     <t>Param</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>AAA,CCC</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>CCCC</t>
+  </si>
+  <si>
+    <t>AAA</t>
   </si>
 </sst>
 </file>
@@ -784,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="F23" s="1">
         <v>2</v>
@@ -1172,7 +1181,7 @@
     </row>
     <row r="67">
       <c r="B67" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>1.0</v>

</xml_diff>